<commit_message>
MAJ URLs SFCC + correctifs UK
</commit_message>
<xml_diff>
--- a/Jeux de donnees/SFCC/New-account/jdd-New-account.xlsx
+++ b/Jeux de donnees/SFCC/New-account/jdd-New-account.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://onepoint365-my.sharepoint.com/personal/s_ramos-izquierdo_groupeonepoint_com/Documents/Bureau/Clarins/Outils/clarins_auto_uat_ihm/Jeux de donnees/SFCC/New-account/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="452" documentId="8_{F2498E7F-A211-5648-BD84-328060702354}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{14FA7A0C-ABF6-4ED2-8F9A-DE5ED9472478}"/>
+  <xr:revisionPtr revIDLastSave="471" documentId="8_{F2498E7F-A211-5648-BD84-328060702354}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{74C9B9C1-2AF9-44B6-92D9-EC174283255D}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{4DDB3DD0-E88E-8949-89B8-E2C45E0A4C00}"/>
   </bookViews>

</xml_diff>

<commit_message>
MAJ JDD NewAccount all YES
</commit_message>
<xml_diff>
--- a/Jeux de donnees/SFCC/New-account/jdd-New-account.xlsx
+++ b/Jeux de donnees/SFCC/New-account/jdd-New-account.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://onepoint365-my.sharepoint.com/personal/s_ramos-izquierdo_groupeonepoint_com/Documents/Bureau/Clarins/Outils/clarins_auto_uat_ihm/Jeux de donnees/SFCC/New-account/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="473" documentId="8_{F2498E7F-A211-5648-BD84-328060702354}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DBBFE260-0A87-45A0-ABCB-1441AE50B741}"/>
+  <xr:revisionPtr revIDLastSave="474" documentId="8_{F2498E7F-A211-5648-BD84-328060702354}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9D1E740F-7ABA-4828-9CE1-FF1167B59CF6}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{4DDB3DD0-E88E-8949-89B8-E2C45E0A4C00}"/>
   </bookViews>
@@ -743,7 +743,7 @@
   <dimension ref="A1:N13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:B9"/>
+      <selection activeCell="B2" sqref="B2:B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.796875" defaultRowHeight="18"/>
@@ -856,7 +856,7 @@
         <v>30</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>6</v>
@@ -898,7 +898,7 @@
         <v>31</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>6</v>
@@ -940,7 +940,7 @@
         <v>32</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>6</v>
@@ -982,7 +982,7 @@
         <v>33</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>6</v>
@@ -1024,7 +1024,7 @@
         <v>34</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>6</v>
@@ -1068,7 +1068,7 @@
         <v>35</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C8" s="6" t="s">
         <v>6</v>
@@ -1112,7 +1112,7 @@
         <v>36</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C9" s="6" t="s">
         <v>6</v>

</xml_diff>

<commit_message>
Correction tests auto NewAccount
</commit_message>
<xml_diff>
--- a/Jeux de donnees/SFCC/New-account/jdd-New-account.xlsx
+++ b/Jeux de donnees/SFCC/New-account/jdd-New-account.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://onepoint365-my.sharepoint.com/personal/s_ramos-izquierdo_groupeonepoint_com/Documents/Bureau/Clarins/Outils/clarins_auto_uat_ihm/Jeux de donnees/SFCC/New-account/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="476" documentId="8_{F2498E7F-A211-5648-BD84-328060702354}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F9494E8F-913A-4F70-87ED-AF174FB4DE9B}"/>
+  <xr:revisionPtr revIDLastSave="484" documentId="8_{F2498E7F-A211-5648-BD84-328060702354}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8D8608C9-E52F-4D81-A0FB-54830DEBCF02}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{4DDB3DD0-E88E-8949-89B8-E2C45E0A4C00}"/>
   </bookViews>
@@ -814,7 +814,7 @@
         <v>29</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>6</v>
@@ -856,7 +856,7 @@
         <v>30</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>6</v>
@@ -898,7 +898,7 @@
         <v>31</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>6</v>
@@ -940,7 +940,7 @@
         <v>32</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>6</v>
@@ -982,7 +982,7 @@
         <v>33</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>6</v>
@@ -1024,7 +1024,7 @@
         <v>34</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>6</v>
@@ -1068,7 +1068,7 @@
         <v>35</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C8" s="6" t="s">
         <v>6</v>
@@ -1112,7 +1112,7 @@
         <v>36</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C9" s="6" t="s">
         <v>6</v>

</xml_diff>